<commit_message>
making this look prettier
and functional
</commit_message>
<xml_diff>
--- a/cmd/GUI/Results.xlsx
+++ b/cmd/GUI/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>File name</t>
   </si>
@@ -37,31 +37,6 @@
   </si>
   <si>
     <t>Char 4 DPS</t>
-  </si>
-  <si>
-    <t>fischl.txt</t>
-  </si>
-  <si>
-    <t>47800.86</t>
-  </si>
-  <si>
-    <t>794.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hutao:
-23432.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xingqiu:
-9744.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yaemiko:
-7834.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fischl:
-6790.36</t>
   </si>
 </sst>
 </file>
@@ -431,7 +406,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -462,29 +437,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>